<commit_message>
start to add dol
</commit_message>
<xml_diff>
--- a/data/DONNEES DOUANE PYTHON.xlsx
+++ b/data/DONNEES DOUANE PYTHON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_Data_Scientist\adam_facture\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782A0440-3377-43D3-AE77-B3EE90F69596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3B3C59-0BAE-4CAC-A481-58B80115FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="156" windowWidth="23040" windowHeight="15552" activeTab="1" xr2:uid="{1FD75016-A00C-4D20-BE15-4A1B0931F8AE}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>NOM STE</t>
   </si>
@@ -251,13 +251,25 @@
   <si>
     <t>Débardeur</t>
     <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAGUE</t>
+  </si>
+  <si>
+    <t>BROCHE</t>
+  </si>
+  <si>
+    <t>BRACELET</t>
+  </si>
+  <si>
+    <t>BOUCLE D'OREILLES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +320,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -329,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -382,12 +400,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,6 +459,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal 1" xfId="1" xr:uid="{E00CF652-13B2-4773-AAE9-9218CD5DDD4E}"/>
@@ -785,15 +842,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EA7AF2-AA55-4AC8-863C-5462B8AA831B}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.44140625" style="6"/>
@@ -1196,7 +1253,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B37" s="8">
@@ -1204,6 +1261,50 @@
       </c>
       <c r="C37" s="8">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="7">
+        <v>62171000</v>
+      </c>
+      <c r="C38" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="7">
+        <v>62171000</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="7">
+        <v>71171910</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="7">
+        <v>62171000</v>
+      </c>
+      <c r="C41" s="7">
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data file: modify DONNEES DOUANE PYTHON.xlsx
</commit_message>
<xml_diff>
--- a/data/DONNEES DOUANE PYTHON.xlsx
+++ b/data/DONNEES DOUANE PYTHON.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_Data_Scientist\adam_facture\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3D9014-9EA8-4032-A9D6-B1F41C2FF6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFC2415-5753-4396-89E6-4264CF9A2834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="23040" windowHeight="15552" activeTab="1" xr2:uid="{1FD75016-A00C-4D20-BE15-4A1B0931F8AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{1FD75016-A00C-4D20-BE15-4A1B0931F8AE}"/>
   </bookViews>
   <sheets>
     <sheet name="STE+NO HABILITE" sheetId="1" r:id="rId1"/>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EA7AF2-AA55-4AC8-863C-5462B8AA831B}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -885,10 +885,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="7">
-        <v>62171000</v>
+        <v>42023290</v>
       </c>
       <c r="C2" s="7">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,10 +1017,10 @@
         <v>57</v>
       </c>
       <c r="B14" s="7">
-        <v>71162011</v>
+        <v>71171900</v>
       </c>
       <c r="C14" s="7">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,10 +1072,10 @@
         <v>67</v>
       </c>
       <c r="B19" s="7">
-        <v>62171000</v>
+        <v>42023290</v>
       </c>
       <c r="C19" s="7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1149,10 +1149,10 @@
         <v>68</v>
       </c>
       <c r="B26" s="7">
-        <v>62171000</v>
+        <v>42023290</v>
       </c>
       <c r="C26" s="7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,7 @@
       <c r="B38" s="7">
         <v>71171900</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="7">
         <v>0.15</v>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       <c r="B39" s="7">
         <v>71171900</v>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="7">
         <v>0.15</v>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       <c r="B40" s="7">
         <v>71171900</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="7">
         <v>0.15</v>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
       <c r="B41" s="7">
         <v>71171900</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="7">
         <v>0.15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance destination country checks in DolvikaFactureReader to include GB and update logging messages
</commit_message>
<xml_diff>
--- a/data/DONNEES DOUANE PYTHON.xlsx
+++ b/data/DONNEES DOUANE PYTHON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_Data_Scientist\adam_facture\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFC2415-5753-4396-89E6-4264CF9A2834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D466AF8-9E69-4EF2-9807-29AA96E47654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{1FD75016-A00C-4D20-BE15-4A1B0931F8AE}"/>
   </bookViews>
@@ -231,9 +231,6 @@
     <t>CHEMISIER</t>
   </si>
   <si>
-    <t>FOURRUE</t>
-  </si>
-  <si>
     <t>PARFUM</t>
   </si>
   <si>
@@ -275,6 +272,10 @@
   </si>
   <si>
     <t>PRESENTOIR</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>FOURRUE</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -857,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EA7AF2-AA55-4AC8-863C-5462B8AA831B}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -885,7 +886,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="7">
-        <v>42023290</v>
+        <v>33030010</v>
       </c>
       <c r="C2" s="7">
         <v>0.05</v>
@@ -915,7 +916,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="7">
         <v>62089900</v>
@@ -1025,7 +1026,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="7">
         <v>62042990</v>
@@ -1036,7 +1037,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7">
         <v>62022000</v>
@@ -1069,13 +1070,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B19" s="7">
-        <v>42023290</v>
+        <v>33030010</v>
       </c>
       <c r="C19" s="7">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,13 +1147,13 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="7">
-        <v>42023290</v>
+        <v>33030010</v>
       </c>
       <c r="C26" s="7">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,7 +1224,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="7">
         <v>61099090</v>
@@ -1267,7 +1268,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="8">
         <v>62089900</v>
@@ -1278,7 +1279,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="7">
         <v>71171900</v>
@@ -1289,7 +1290,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="7">
         <v>71171900</v>
@@ -1300,7 +1301,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" s="7">
         <v>71171900</v>
@@ -1311,7 +1312,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" s="7">
         <v>71171900</v>
@@ -1322,7 +1323,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="7">
         <v>42023210</v>
@@ -1333,7 +1334,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="7">
         <v>39269097</v>
@@ -1344,7 +1345,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="7">
         <v>44219910</v>

</xml_diff>